<commit_message>
Folder name issue resolve
</commit_message>
<xml_diff>
--- a/uploads/BrainerHubAssignmentSheet.xlsx
+++ b/uploads/BrainerHubAssignmentSheet.xlsx
@@ -489,13 +489,13 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>47473.73</v>
+        <v>32782.94</v>
       </c>
       <c r="G2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -523,13 +523,13 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>32760.29</v>
+        <v>64783.93</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -557,10 +557,10 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>87990.32000000001</v>
+        <v>68844.25</v>
       </c>
       <c r="G4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -591,13 +591,13 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>33148.76</v>
+        <v>92570.64</v>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -625,13 +625,13 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>38895.77</v>
+        <v>76810.39999999999</v>
       </c>
       <c r="G6" t="n">
         <v>5</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>44274.82</v>
+        <v>77706.64</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -693,13 +693,13 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>56174.44</v>
+        <v>93011.63</v>
       </c>
       <c r="G8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H8" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -727,13 +727,13 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>59401.7</v>
+        <v>87330.58</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -761,13 +761,13 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>32722.13</v>
+        <v>51216.11</v>
       </c>
       <c r="G10" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H10" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -795,13 +795,13 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>63905.57</v>
+        <v>54035.1</v>
       </c>
       <c r="G11" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -829,13 +829,13 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>63866.08</v>
+        <v>84947.84</v>
       </c>
       <c r="G12" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H12" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -863,13 +863,13 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>62126.72</v>
+        <v>46564.92</v>
       </c>
       <c r="G13" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H13" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
@@ -897,10 +897,10 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>37323.42</v>
+        <v>36589.02</v>
       </c>
       <c r="G14" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H14" t="n">
         <v>5</v>
@@ -931,10 +931,10 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>83774.57000000001</v>
+        <v>52951.43</v>
       </c>
       <c r="G15" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H15" t="n">
         <v>3</v>
@@ -965,13 +965,13 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>81969.62</v>
+        <v>34252.34</v>
       </c>
       <c r="G16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H16" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
@@ -999,10 +999,10 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>86554.27</v>
+        <v>35251.46</v>
       </c>
       <c r="G17" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H17" t="n">
         <v>5</v>
@@ -1033,13 +1033,13 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>77671.78</v>
+        <v>53432.94</v>
       </c>
       <c r="G18" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H18" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -1067,13 +1067,13 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>31882.2</v>
+        <v>93101.91</v>
       </c>
       <c r="G19" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H19" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -1101,13 +1101,13 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>68152.86</v>
+        <v>46310.09</v>
       </c>
       <c r="G20" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -1135,13 +1135,13 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>94676.88</v>
+        <v>69783.53</v>
       </c>
       <c r="G21" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
@@ -1169,13 +1169,13 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>30447.54</v>
+        <v>62239.46</v>
       </c>
       <c r="G22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H22" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -1203,13 +1203,13 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>70520.25999999999</v>
+        <v>66203.67</v>
       </c>
       <c r="G23" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
@@ -1237,10 +1237,10 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>72956.64</v>
+        <v>33779.86</v>
       </c>
       <c r="G24" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H24" t="n">
         <v>4</v>
@@ -1271,13 +1271,13 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>80113.21000000001</v>
+        <v>68757.35000000001</v>
       </c>
       <c r="G25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1305,13 +1305,13 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>33437.5</v>
+        <v>68970.78999999999</v>
       </c>
       <c r="G26" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H26" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27">
@@ -1339,10 +1339,10 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>68923.63</v>
+        <v>66939.73</v>
       </c>
       <c r="G27" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H27" t="n">
         <v>4</v>
@@ -1373,13 +1373,13 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>50744.48</v>
+        <v>82147.63</v>
       </c>
       <c r="G28" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H28" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
@@ -1407,13 +1407,13 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>83722.53</v>
+        <v>68103.28999999999</v>
       </c>
       <c r="G29" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H29" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
@@ -1441,13 +1441,13 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>62181.05</v>
+        <v>66163.17999999999</v>
       </c>
       <c r="G30" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1475,13 +1475,13 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>62237.39</v>
+        <v>80505.92</v>
       </c>
       <c r="G31" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H31" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
@@ -1509,13 +1509,13 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>33350.78</v>
+        <v>92134.13</v>
       </c>
       <c r="G32" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H32" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33">
@@ -1543,13 +1543,13 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>60335.28</v>
+        <v>77663.71000000001</v>
       </c>
       <c r="G33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H33" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34">
@@ -1577,10 +1577,10 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>76642.48</v>
+        <v>93058.49000000001</v>
       </c>
       <c r="G34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H34" t="n">
         <v>3</v>
@@ -1611,13 +1611,13 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>46805.25</v>
+        <v>48891.26</v>
       </c>
       <c r="G35" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H35" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36">
@@ -1645,13 +1645,13 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>99993.94</v>
+        <v>64729.06</v>
       </c>
       <c r="G36" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H36" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
@@ -1679,10 +1679,10 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>88849.34</v>
+        <v>40100.87</v>
       </c>
       <c r="G37" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H37" t="n">
         <v>3</v>
@@ -1713,10 +1713,10 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>33736.41</v>
+        <v>65327.75</v>
       </c>
       <c r="G38" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H38" t="n">
         <v>2</v>
@@ -1747,13 +1747,13 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>63240.51</v>
+        <v>70823.73</v>
       </c>
       <c r="G39" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -1781,13 +1781,13 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>64889.27</v>
+        <v>72342.36</v>
       </c>
       <c r="G40" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -1815,13 +1815,13 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>69390.75</v>
+        <v>73821.23</v>
       </c>
       <c r="G41" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
@@ -1849,13 +1849,13 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>74781.03999999999</v>
+        <v>43829.72</v>
       </c>
       <c r="G42" t="n">
         <v>6</v>
       </c>
       <c r="H42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
@@ -1883,13 +1883,13 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>45078.9</v>
+        <v>73465.78</v>
       </c>
       <c r="G43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H43" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">
@@ -1917,13 +1917,13 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>54762.65</v>
+        <v>39704.67</v>
       </c>
       <c r="G44" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H44" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45">
@@ -1951,13 +1951,13 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>39499.86</v>
+        <v>70345.73</v>
       </c>
       <c r="G45" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H45" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46">
@@ -1985,13 +1985,13 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>79161.12</v>
+        <v>81879.17</v>
       </c>
       <c r="G46" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H46" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47">
@@ -2019,10 +2019,10 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>57467.67</v>
+        <v>97245.82000000001</v>
       </c>
       <c r="G47" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H47" t="n">
         <v>5</v>
@@ -2053,13 +2053,13 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>43032.46</v>
+        <v>79261.56</v>
       </c>
       <c r="G48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H48" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49">
@@ -2087,13 +2087,13 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>41814.13</v>
+        <v>47033.56</v>
       </c>
       <c r="G49" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H49" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
@@ -2121,13 +2121,13 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>81699.03</v>
+        <v>73037.24000000001</v>
       </c>
       <c r="G50" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H50" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51">
@@ -2155,10 +2155,10 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>90907.96000000001</v>
+        <v>38587.91</v>
       </c>
       <c r="G51" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H51" t="n">
         <v>5</v>
@@ -2189,13 +2189,13 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>92802.14999999999</v>
+        <v>65352.76</v>
       </c>
       <c r="G52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H52" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53">
@@ -2223,13 +2223,13 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>56116.37</v>
+        <v>44261.35</v>
       </c>
       <c r="G53" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54">
@@ -2257,10 +2257,10 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>55723.06</v>
+        <v>36295.76</v>
       </c>
       <c r="G54" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H54" t="n">
         <v>2</v>
@@ -2291,10 +2291,10 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>76115.62</v>
+        <v>67410.72</v>
       </c>
       <c r="G55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H55" t="n">
         <v>1</v>
@@ -2325,13 +2325,13 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>47338.81</v>
+        <v>30463.77</v>
       </c>
       <c r="G56" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H56" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57">
@@ -2359,13 +2359,13 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>92811.84</v>
+        <v>37704.98</v>
       </c>
       <c r="G57" t="n">
         <v>7</v>
       </c>
       <c r="H57" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58">
@@ -2393,13 +2393,13 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>50837.19</v>
+        <v>45808.88</v>
       </c>
       <c r="G58" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H58" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59">
@@ -2427,10 +2427,10 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>43409.73</v>
+        <v>64630.3</v>
       </c>
       <c r="G59" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H59" t="n">
         <v>5</v>
@@ -2461,13 +2461,13 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>99427.50999999999</v>
+        <v>88981.64999999999</v>
       </c>
       <c r="G60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H60" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
@@ -2495,13 +2495,13 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>66165.09</v>
+        <v>86762.95</v>
       </c>
       <c r="G61" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62">
@@ -2529,13 +2529,13 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>98858.87</v>
+        <v>55374.25</v>
       </c>
       <c r="G62" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H62" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63">
@@ -2563,13 +2563,13 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>72103.14999999999</v>
+        <v>44478.14</v>
       </c>
       <c r="G63" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H63" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -2597,10 +2597,10 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>47242.52</v>
+        <v>44659.69</v>
       </c>
       <c r="G64" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H64" t="n">
         <v>5</v>
@@ -2631,13 +2631,13 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>75179.88</v>
+        <v>50189.87</v>
       </c>
       <c r="G65" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H65" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -2665,7 +2665,7 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>64602.58</v>
+        <v>85888.91</v>
       </c>
       <c r="G66" t="n">
         <v>4</v>
@@ -2699,13 +2699,13 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>59753.13</v>
+        <v>71546.86</v>
       </c>
       <c r="G67" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -2733,13 +2733,13 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>42110.63</v>
+        <v>49673.93</v>
       </c>
       <c r="G68" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H68" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -2767,13 +2767,13 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>88161.17</v>
+        <v>52075.79</v>
       </c>
       <c r="G69" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H69" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70">
@@ -2801,13 +2801,13 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>45220.64</v>
+        <v>95359.23</v>
       </c>
       <c r="G70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
@@ -2835,13 +2835,13 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>49719.12</v>
+        <v>89207.82000000001</v>
       </c>
       <c r="G71" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H71" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72">
@@ -2869,13 +2869,13 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>65717.17999999999</v>
+        <v>86615.09</v>
       </c>
       <c r="G72" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -2903,10 +2903,10 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>48137.45</v>
+        <v>86711.21000000001</v>
       </c>
       <c r="G73" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H73" t="n">
         <v>5</v>
@@ -2937,13 +2937,13 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>54972.74</v>
+        <v>58254.1</v>
       </c>
       <c r="G74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H74" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75">
@@ -2971,13 +2971,13 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>35339.16</v>
+        <v>59893.33</v>
       </c>
       <c r="G75" t="n">
         <v>10</v>
       </c>
       <c r="H75" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76">
@@ -3005,10 +3005,10 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>44565.83</v>
+        <v>30389.22</v>
       </c>
       <c r="G76" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H76" t="n">
         <v>5</v>
@@ -3039,13 +3039,13 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>33231.38</v>
+        <v>46985.51</v>
       </c>
       <c r="G77" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H77" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78">
@@ -3073,13 +3073,13 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>39890.12</v>
+        <v>90303.08</v>
       </c>
       <c r="G78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H78" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79">
@@ -3107,13 +3107,13 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>62732.02</v>
+        <v>83861.98</v>
       </c>
       <c r="G79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H79" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80">
@@ -3141,13 +3141,13 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>76357.88</v>
+        <v>95595</v>
       </c>
       <c r="G80" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H80" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81">
@@ -3175,13 +3175,13 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>59727.29</v>
+        <v>87752.85000000001</v>
       </c>
       <c r="G81" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H81" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -3209,13 +3209,13 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>77795.48</v>
+        <v>61722.04</v>
       </c>
       <c r="G82" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H82" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83">
@@ -3243,13 +3243,13 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>40970.66</v>
+        <v>49537.94</v>
       </c>
       <c r="G83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H83" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -3277,13 +3277,13 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>76585.25999999999</v>
+        <v>76340.49000000001</v>
       </c>
       <c r="G84" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H84" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85">
@@ -3311,13 +3311,13 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>72324.47</v>
+        <v>68742.64999999999</v>
       </c>
       <c r="G85" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H85" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86">
@@ -3345,13 +3345,13 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>82566.24000000001</v>
+        <v>36911.73</v>
       </c>
       <c r="G86" t="n">
         <v>6</v>
       </c>
       <c r="H86" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87">
@@ -3379,13 +3379,13 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>67481.10000000001</v>
+        <v>81207.81</v>
       </c>
       <c r="G87" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H87" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88">
@@ -3413,13 +3413,13 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>52121.29</v>
+        <v>43349.55</v>
       </c>
       <c r="G88" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H88" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89">
@@ -3447,10 +3447,10 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>63772.3</v>
+        <v>90515.27</v>
       </c>
       <c r="G89" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H89" t="n">
         <v>4</v>
@@ -3481,13 +3481,13 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>89710.97</v>
+        <v>36473.26</v>
       </c>
       <c r="G90" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H90" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -3515,10 +3515,10 @@
         </is>
       </c>
       <c r="F91" t="n">
-        <v>71343.22</v>
+        <v>57243.91</v>
       </c>
       <c r="G91" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H91" t="n">
         <v>2</v>
@@ -3549,13 +3549,13 @@
         </is>
       </c>
       <c r="F92" t="n">
-        <v>98033.50999999999</v>
+        <v>40745.12</v>
       </c>
       <c r="G92" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
@@ -3583,7 +3583,7 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>93580.82000000001</v>
+        <v>54512.92</v>
       </c>
       <c r="G93" t="n">
         <v>1</v>
@@ -3617,13 +3617,13 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>80677.8</v>
+        <v>35942.48</v>
       </c>
       <c r="G94" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H94" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95">
@@ -3651,10 +3651,10 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>36625.33</v>
+        <v>51157.87</v>
       </c>
       <c r="G95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H95" t="n">
         <v>2</v>
@@ -3685,10 +3685,10 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>86272.98</v>
+        <v>46048.21</v>
       </c>
       <c r="G96" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H96" t="n">
         <v>2</v>
@@ -3719,13 +3719,13 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>87591.8</v>
+        <v>94677.07000000001</v>
       </c>
       <c r="G97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H97" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98">
@@ -3753,13 +3753,13 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>32243.13</v>
+        <v>62024.31</v>
       </c>
       <c r="G98" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H98" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99">
@@ -3787,10 +3787,10 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>96286.34</v>
+        <v>68702.19</v>
       </c>
       <c r="G99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H99" t="n">
         <v>2</v>
@@ -3821,13 +3821,13 @@
         </is>
       </c>
       <c r="F100" t="n">
-        <v>90259.50999999999</v>
+        <v>74990.98</v>
       </c>
       <c r="G100" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H100" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101">
@@ -3855,10 +3855,10 @@
         </is>
       </c>
       <c r="F101" t="n">
-        <v>97381.37</v>
+        <v>62288.6</v>
       </c>
       <c r="G101" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H101" t="n">
         <v>2</v>
@@ -3912,10 +3912,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>47473.73</v>
+        <v>32782.94</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>2</v>
@@ -3928,10 +3928,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>32760.29</v>
+        <v>64783.93</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
         <v>4</v>
@@ -3944,13 +3944,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>87990.32000000001</v>
+        <v>68844.25</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -3960,13 +3960,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>33148.76</v>
+        <v>92570.64</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -3976,10 +3976,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>38895.77</v>
+        <v>76810.39999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="n">
         <v>2</v>
@@ -3992,13 +3992,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>44274.82</v>
+        <v>77706.64</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -4008,13 +4008,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>56174.44</v>
+        <v>93011.63</v>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -4024,10 +4024,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>59401.7</v>
+        <v>87330.58</v>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" t="n">
         <v>2</v>
@@ -4040,13 +4040,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>32722.13</v>
+        <v>51216.11</v>
       </c>
       <c r="C10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" t="n">
         <v>2</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -4056,13 +4056,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>63905.57</v>
+        <v>54035.1</v>
       </c>
       <c r="C11" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -4072,13 +4072,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>63866.08</v>
+        <v>84947.84</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
@@ -4088,13 +4088,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>62126.72</v>
+        <v>46564.92</v>
       </c>
       <c r="C13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
@@ -4104,10 +4104,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>37323.42</v>
+        <v>36589.02</v>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
         <v>3</v>
@@ -4120,13 +4120,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>83774.57000000001</v>
+        <v>52951.43</v>
       </c>
       <c r="C15" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D15" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -4136,10 +4136,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>81969.62</v>
+        <v>34252.34</v>
       </c>
       <c r="C16" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
         <v>2</v>
@@ -4152,10 +4152,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>86554.27</v>
+        <v>35251.46</v>
       </c>
       <c r="C17" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
         <v>4</v>
@@ -4168,13 +4168,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>77671.78</v>
+        <v>53432.94</v>
       </c>
       <c r="C18" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -4184,10 +4184,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>31882.2</v>
+        <v>93101.91</v>
       </c>
       <c r="C19" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
         <v>3</v>
@@ -4200,13 +4200,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>68152.86</v>
+        <v>46310.09</v>
       </c>
       <c r="C20" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -4216,13 +4216,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>94676.88</v>
+        <v>69783.53</v>
       </c>
       <c r="C21" t="n">
         <v>2</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
@@ -4232,13 +4232,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>30447.54</v>
+        <v>62239.46</v>
       </c>
       <c r="C22" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
@@ -4248,13 +4248,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>70520.25999999999</v>
+        <v>66203.67</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
@@ -4264,13 +4264,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>72956.64</v>
+        <v>33779.86</v>
       </c>
       <c r="C24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D24" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -4280,13 +4280,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>80113.21000000001</v>
+        <v>68757.35000000001</v>
       </c>
       <c r="C25" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D25" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>33437.5</v>
+        <v>68970.78999999999</v>
       </c>
       <c r="C26" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D26" t="n">
         <v>4</v>
@@ -4312,10 +4312,10 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>68923.63</v>
+        <v>66939.73</v>
       </c>
       <c r="C27" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D27" t="n">
         <v>1</v>
@@ -4328,13 +4328,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>50744.48</v>
+        <v>82147.63</v>
       </c>
       <c r="C28" t="n">
+        <v>5</v>
+      </c>
+      <c r="D28" t="n">
         <v>2</v>
-      </c>
-      <c r="D28" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="29">
@@ -4344,13 +4344,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>83722.53</v>
+        <v>68103.28999999999</v>
       </c>
       <c r="C29" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30">
@@ -4360,10 +4360,10 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>62181.05</v>
+        <v>66163.17999999999</v>
       </c>
       <c r="C30" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D30" t="n">
         <v>4</v>
@@ -4376,10 +4376,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>62237.39</v>
+        <v>80505.92</v>
       </c>
       <c r="C31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31" t="n">
         <v>5</v>
@@ -4392,13 +4392,13 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>33350.78</v>
+        <v>92134.13</v>
       </c>
       <c r="C32" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D32" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -4408,13 +4408,13 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>60335.28</v>
+        <v>77663.71000000001</v>
       </c>
       <c r="C33" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34">
@@ -4424,13 +4424,13 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>76642.48</v>
+        <v>93058.49000000001</v>
       </c>
       <c r="C34" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D34" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -4440,10 +4440,10 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>46805.25</v>
+        <v>48891.26</v>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D35" t="n">
         <v>2</v>
@@ -4456,13 +4456,13 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>99993.94</v>
+        <v>64729.06</v>
       </c>
       <c r="C36" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D36" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -4472,13 +4472,13 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>88849.34</v>
+        <v>40100.87</v>
       </c>
       <c r="C37" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D37" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38">
@@ -4488,13 +4488,13 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>33736.41</v>
+        <v>65327.75</v>
       </c>
       <c r="C38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D38" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -4504,13 +4504,13 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>63240.51</v>
+        <v>70823.73</v>
       </c>
       <c r="C39" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -4520,13 +4520,13 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>64889.27</v>
+        <v>72342.36</v>
       </c>
       <c r="C40" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D40" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41">
@@ -4536,13 +4536,13 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>69390.75</v>
+        <v>73821.23</v>
       </c>
       <c r="C41" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D41" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
@@ -4552,13 +4552,13 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>74781.03999999999</v>
+        <v>43829.72</v>
       </c>
       <c r="C42" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D42" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
@@ -4568,13 +4568,13 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>45078.9</v>
+        <v>73465.78</v>
       </c>
       <c r="C43" t="n">
         <v>3</v>
       </c>
       <c r="D43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">
@@ -4584,13 +4584,13 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>54762.65</v>
+        <v>39704.67</v>
       </c>
       <c r="C44" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D44" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45">
@@ -4600,13 +4600,13 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>39499.86</v>
+        <v>70345.73</v>
       </c>
       <c r="C45" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46">
@@ -4616,13 +4616,13 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>79161.12</v>
+        <v>81879.17</v>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D46" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47">
@@ -4632,13 +4632,13 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>57467.67</v>
+        <v>97245.82000000001</v>
       </c>
       <c r="C47" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D47" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -4648,13 +4648,13 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>43032.46</v>
+        <v>79261.56</v>
       </c>
       <c r="C48" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D48" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
@@ -4664,13 +4664,13 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>41814.13</v>
+        <v>47033.56</v>
       </c>
       <c r="C49" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D49" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
@@ -4680,13 +4680,13 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>81699.03</v>
+        <v>73037.24000000001</v>
       </c>
       <c r="C50" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -4696,13 +4696,13 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>90907.96000000001</v>
+        <v>38587.91</v>
       </c>
       <c r="C51" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D51" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52">
@@ -4712,13 +4712,13 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>92802.14999999999</v>
+        <v>65352.76</v>
       </c>
       <c r="C52" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53">
@@ -4728,13 +4728,13 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>56116.37</v>
+        <v>44261.35</v>
       </c>
       <c r="C53" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D53" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54">
@@ -4744,13 +4744,13 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>55723.06</v>
+        <v>36295.76</v>
       </c>
       <c r="C54" t="n">
         <v>4</v>
       </c>
       <c r="D54" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55">
@@ -4760,13 +4760,13 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>76115.62</v>
+        <v>67410.72</v>
       </c>
       <c r="C55" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56">
@@ -4776,13 +4776,13 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>47338.81</v>
+        <v>30463.77</v>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
@@ -4792,13 +4792,13 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>92811.84</v>
+        <v>37704.98</v>
       </c>
       <c r="C57" t="n">
+        <v>8</v>
+      </c>
+      <c r="D57" t="n">
         <v>1</v>
-      </c>
-      <c r="D57" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="58">
@@ -4808,10 +4808,10 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>50837.19</v>
+        <v>45808.88</v>
       </c>
       <c r="C58" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D58" t="n">
         <v>3</v>
@@ -4824,10 +4824,10 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>43409.73</v>
+        <v>64630.3</v>
       </c>
       <c r="C59" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D59" t="n">
         <v>2</v>
@@ -4840,13 +4840,13 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>99427.50999999999</v>
+        <v>88981.64999999999</v>
       </c>
       <c r="C60" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -4856,13 +4856,13 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>66165.09</v>
+        <v>86762.95</v>
       </c>
       <c r="C61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D61" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
@@ -4872,13 +4872,13 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>98858.87</v>
+        <v>55374.25</v>
       </c>
       <c r="C62" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D62" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63">
@@ -4888,13 +4888,13 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>72103.14999999999</v>
+        <v>44478.14</v>
       </c>
       <c r="C63" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D63" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64">
@@ -4904,13 +4904,13 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>47242.52</v>
+        <v>44659.69</v>
       </c>
       <c r="C64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D64" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65">
@@ -4920,13 +4920,13 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>75179.88</v>
+        <v>50189.87</v>
       </c>
       <c r="C65" t="n">
         <v>4</v>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66">
@@ -4936,10 +4936,10 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>64602.58</v>
+        <v>85888.91</v>
       </c>
       <c r="C66" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D66" t="n">
         <v>5</v>
@@ -4952,10 +4952,10 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>59753.13</v>
+        <v>71546.86</v>
       </c>
       <c r="C67" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D67" t="n">
         <v>1</v>
@@ -4968,7 +4968,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>42110.63</v>
+        <v>49673.93</v>
       </c>
       <c r="C68" t="n">
         <v>4</v>
@@ -4984,13 +4984,13 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>88161.17</v>
+        <v>52075.79</v>
       </c>
       <c r="C69" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70">
@@ -5000,13 +5000,13 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>45220.64</v>
+        <v>95359.23</v>
       </c>
       <c r="C70" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -5016,13 +5016,13 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>49719.12</v>
+        <v>89207.82000000001</v>
       </c>
       <c r="C71" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D71" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -5032,13 +5032,13 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>65717.17999999999</v>
+        <v>86615.09</v>
       </c>
       <c r="C72" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D72" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -5048,10 +5048,10 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>48137.45</v>
+        <v>86711.21000000001</v>
       </c>
       <c r="C73" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D73" t="n">
         <v>4</v>
@@ -5064,13 +5064,13 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>54972.74</v>
+        <v>58254.1</v>
       </c>
       <c r="C74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
@@ -5080,13 +5080,13 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>35339.16</v>
+        <v>59893.33</v>
       </c>
       <c r="C75" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76">
@@ -5096,13 +5096,13 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>44565.83</v>
+        <v>30389.22</v>
       </c>
       <c r="C76" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D76" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -5112,13 +5112,13 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>33231.38</v>
+        <v>46985.51</v>
       </c>
       <c r="C77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78">
@@ -5128,13 +5128,13 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>39890.12</v>
+        <v>90303.08</v>
       </c>
       <c r="C78" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D78" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79">
@@ -5144,13 +5144,13 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>62732.02</v>
+        <v>83861.98</v>
       </c>
       <c r="C79" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D79" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80">
@@ -5160,13 +5160,13 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>76357.88</v>
+        <v>95595</v>
       </c>
       <c r="C80" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D80" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -5176,13 +5176,13 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>59727.29</v>
+        <v>87752.85000000001</v>
       </c>
       <c r="C81" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D81" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82">
@@ -5192,13 +5192,13 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>77795.48</v>
+        <v>61722.04</v>
       </c>
       <c r="C82" t="n">
         <v>5</v>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83">
@@ -5208,13 +5208,13 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>40970.66</v>
+        <v>49537.94</v>
       </c>
       <c r="C83" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D83" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84">
@@ -5224,10 +5224,10 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>76585.25999999999</v>
+        <v>76340.49000000001</v>
       </c>
       <c r="C84" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D84" t="n">
         <v>1</v>
@@ -5240,13 +5240,13 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>72324.47</v>
+        <v>68742.64999999999</v>
       </c>
       <c r="C85" t="n">
+        <v>3</v>
+      </c>
+      <c r="D85" t="n">
         <v>1</v>
-      </c>
-      <c r="D85" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="86">
@@ -5256,13 +5256,13 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>82566.24000000001</v>
+        <v>36911.73</v>
       </c>
       <c r="C86" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D86" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87">
@@ -5272,13 +5272,13 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>67481.10000000001</v>
+        <v>81207.81</v>
       </c>
       <c r="C87" t="n">
         <v>4</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88">
@@ -5288,13 +5288,13 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>52121.29</v>
+        <v>43349.55</v>
       </c>
       <c r="C88" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D88" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89">
@@ -5304,13 +5304,13 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>63772.3</v>
+        <v>90515.27</v>
       </c>
       <c r="C89" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D89" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90">
@@ -5320,13 +5320,13 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>89710.97</v>
+        <v>36473.26</v>
       </c>
       <c r="C90" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D90" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -5336,13 +5336,13 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>71343.22</v>
+        <v>57243.91</v>
       </c>
       <c r="C91" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D91" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -5352,13 +5352,13 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>98033.50999999999</v>
+        <v>40745.12</v>
       </c>
       <c r="C92" t="n">
         <v>2</v>
       </c>
       <c r="D92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
@@ -5368,13 +5368,13 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>93580.82000000001</v>
+        <v>54512.92</v>
       </c>
       <c r="C93" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
@@ -5384,13 +5384,13 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>80677.8</v>
+        <v>35942.48</v>
       </c>
       <c r="C94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95">
@@ -5400,13 +5400,13 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>36625.33</v>
+        <v>51157.87</v>
       </c>
       <c r="C95" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D95" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96">
@@ -5416,13 +5416,13 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>86272.98</v>
+        <v>46048.21</v>
       </c>
       <c r="C96" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D96" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97">
@@ -5432,13 +5432,13 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>87591.8</v>
+        <v>94677.07000000001</v>
       </c>
       <c r="C97" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D97" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98">
@@ -5448,13 +5448,13 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>32243.13</v>
+        <v>62024.31</v>
       </c>
       <c r="C98" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D98" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99">
@@ -5464,13 +5464,13 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>96286.34</v>
+        <v>68702.19</v>
       </c>
       <c r="C99" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100">
@@ -5480,13 +5480,13 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>90259.50999999999</v>
+        <v>74990.98</v>
       </c>
       <c r="C100" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D100" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101">
@@ -5496,13 +5496,13 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>97381.37</v>
+        <v>62288.6</v>
       </c>
       <c r="C101" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D101" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>